<commit_message>
Add secondary instructors to courses
</commit_message>
<xml_diff>
--- a/FinalExamScheduling/FinalExamScheduling/Input2.xlsx
+++ b/FinalExamScheduling/FinalExamScheduling/Input2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BME\Beosztástervezés\schedule\FinalExamScheduling\FinalExamScheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7040CCEB-2084-4CA5-AACD-16B88B2D9175}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77380F7-0F93-490F-B477-BAF5B5256DEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="3915" windowWidth="20730" windowHeight="11160" tabRatio="686" activeTab="3" xr2:uid="{50175455-BC8E-4A3E-9C2C-228FA398DDE4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="686" xr2:uid="{50175455-BC8E-4A3E-9C2C-228FA398DDE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="5" r:id="rId1"/>
@@ -2187,8 +2187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA1CCB9-2E77-407B-8403-9B3763A1995B}">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2471,7 +2471,7 @@
         <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D12" t="s">
         <v>272</v>
@@ -4927,7 +4927,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18899,9 +18899,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7CDAB86-CB84-4B22-91BD-821B5CA48E47}">
   <dimension ref="A1:BS14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X8" sqref="X8"/>
+      <selection pane="topRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
block handling written, availabilities checked, output ordered, run speeded up
</commit_message>
<xml_diff>
--- a/FinalExamScheduling/FinalExamScheduling/Input2.xlsx
+++ b/FinalExamScheduling/FinalExamScheduling/Input2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BME\Beosztástervezés\schedule\FinalExamScheduling\FinalExamScheduling\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tóni\source\repos\schedule\FinalExamScheduling\FinalExamScheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96CA69B-B112-4261-8C5C-8FD5D993C596}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="686" activeTab="3" xr2:uid="{50175455-BC8E-4A3E-9C2C-228FA398DDE4}"/>
+    <workbookView minimized="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="686"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="5" r:id="rId1"/>
@@ -1305,7 +1304,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
@@ -1747,33 +1746,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="27">
-    <cellStyle name="descriptionStyle" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="descriptionStyle 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="footerStyle" xfId="11" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="footerStyle 2" xfId="23" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="headerCenterDarkStyle" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="headerCenterDarkStyle 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="headerCenterLightStyle" xfId="8" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="headerCenterLightStyle 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="headerLeftDarkStyle" xfId="7" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="headerLeftDarkStyle 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="headerRightLightStyle" xfId="10" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="headerRightLightStyle 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="headerRightStyle" xfId="9" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="headerRightStyle 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="headerStyle" xfId="5" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="headerStyle 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Hyperlink 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="descriptionStyle" xfId="4"/>
+    <cellStyle name="descriptionStyle 2" xfId="16"/>
+    <cellStyle name="footerStyle" xfId="11"/>
+    <cellStyle name="footerStyle 2" xfId="23"/>
+    <cellStyle name="headerCenterDarkStyle" xfId="6"/>
+    <cellStyle name="headerCenterDarkStyle 2" xfId="18"/>
+    <cellStyle name="headerCenterLightStyle" xfId="8"/>
+    <cellStyle name="headerCenterLightStyle 2" xfId="20"/>
+    <cellStyle name="headerLeftDarkStyle" xfId="7"/>
+    <cellStyle name="headerLeftDarkStyle 2" xfId="19"/>
+    <cellStyle name="headerRightLightStyle" xfId="10"/>
+    <cellStyle name="headerRightLightStyle 2" xfId="22"/>
+    <cellStyle name="headerRightStyle" xfId="9"/>
+    <cellStyle name="headerRightStyle 2" xfId="21"/>
+    <cellStyle name="headerStyle" xfId="5"/>
+    <cellStyle name="headerStyle 2" xfId="17"/>
+    <cellStyle name="Hyperlink 2" xfId="24"/>
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Normál 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="Normal 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Normál 3" xfId="25" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="Normál 4" xfId="26" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="subTitleStyle" xfId="3" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="subTitleStyle 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="titleStyle" xfId="2" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="titleStyle 2" xfId="14" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="12"/>
+    <cellStyle name="Normál 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="13"/>
+    <cellStyle name="Normál 3" xfId="25"/>
+    <cellStyle name="Normál 4" xfId="26"/>
+    <cellStyle name="subTitleStyle" xfId="3"/>
+    <cellStyle name="subTitleStyle 2" xfId="15"/>
+    <cellStyle name="titleStyle" xfId="2"/>
+    <cellStyle name="titleStyle 2" xfId="14"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -2189,16 +2188,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FA1CCB9-2E77-407B-8403-9B3763A1995B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -4927,7 +4928,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73052356-DAFD-4478-A49E-D17CE04C86B1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BX84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18291,7 +18292,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2884E5-45FE-41A9-80CC-48E3600DC49D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18854,7 +18855,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="A1:AA6">
+  <sortState columnSort="1" ref="A1:AA6">
     <sortCondition ref="A1:AA1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18862,10 +18863,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7CDAB86-CB84-4B22-91BD-821B5CA48E47}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BS14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="V11" sqref="V11"/>
     </sheetView>

</xml_diff>

<commit_message>
excel-helper read-full fixed (case-insensitivity)
</commit_message>
<xml_diff>
--- a/FinalExamScheduling/FinalExamScheduling/Input2.xlsx
+++ b/FinalExamScheduling/FinalExamScheduling/Input2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tóni\source\repos\schedule\FinalExamScheduling\FinalExamScheduling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\repos\schedule\FinalExamScheduling\FinalExamScheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D7138A-ADDC-463F-9D2F-B73449094111}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="686"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="686" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="5" r:id="rId1"/>
@@ -1304,7 +1305,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
@@ -1746,33 +1747,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="27">
-    <cellStyle name="descriptionStyle" xfId="4"/>
-    <cellStyle name="descriptionStyle 2" xfId="16"/>
-    <cellStyle name="footerStyle" xfId="11"/>
-    <cellStyle name="footerStyle 2" xfId="23"/>
-    <cellStyle name="headerCenterDarkStyle" xfId="6"/>
-    <cellStyle name="headerCenterDarkStyle 2" xfId="18"/>
-    <cellStyle name="headerCenterLightStyle" xfId="8"/>
-    <cellStyle name="headerCenterLightStyle 2" xfId="20"/>
-    <cellStyle name="headerLeftDarkStyle" xfId="7"/>
-    <cellStyle name="headerLeftDarkStyle 2" xfId="19"/>
-    <cellStyle name="headerRightLightStyle" xfId="10"/>
-    <cellStyle name="headerRightLightStyle 2" xfId="22"/>
-    <cellStyle name="headerRightStyle" xfId="9"/>
-    <cellStyle name="headerRightStyle 2" xfId="21"/>
-    <cellStyle name="headerStyle" xfId="5"/>
-    <cellStyle name="headerStyle 2" xfId="17"/>
-    <cellStyle name="Hyperlink 2" xfId="24"/>
+    <cellStyle name="descriptionStyle" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="descriptionStyle 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="footerStyle" xfId="11" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="footerStyle 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="headerCenterDarkStyle" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="headerCenterDarkStyle 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="headerCenterLightStyle" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="headerCenterLightStyle 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="headerLeftDarkStyle" xfId="7" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="headerLeftDarkStyle 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="headerRightLightStyle" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="headerRightLightStyle 2" xfId="22" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="headerRightStyle" xfId="9" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="headerRightStyle 2" xfId="21" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="headerStyle" xfId="5" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="headerStyle 2" xfId="17" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="12"/>
-    <cellStyle name="Normál 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="13"/>
-    <cellStyle name="Normál 3" xfId="25"/>
-    <cellStyle name="Normál 4" xfId="26"/>
-    <cellStyle name="subTitleStyle" xfId="3"/>
-    <cellStyle name="subTitleStyle 2" xfId="15"/>
-    <cellStyle name="titleStyle" xfId="2"/>
-    <cellStyle name="titleStyle 2" xfId="14"/>
+    <cellStyle name="Normal 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normál 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal 3" xfId="13" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normál 3" xfId="25" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Normál 4" xfId="26" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="subTitleStyle" xfId="3" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="subTitleStyle 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="titleStyle" xfId="2" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="titleStyle 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -2188,18 +2189,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -4928,12 +4929,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BX84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA20" sqref="AA20"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A56" sqref="A56:XFD60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18292,7 +18295,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AM8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18855,7 +18858,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState columnSort="1" ref="A1:AA6">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="A1:AA6">
     <sortCondition ref="A1:AA1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18863,7 +18866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BS14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>